<commit_message>
Fix chart errors, style errors, add more examples, minor changes, in progress...
</commit_message>
<xml_diff>
--- a/src/samples/FullFramework/iXlsxWriter.ConsoleApp/Output/Sample-01/Sample-01.xlsx
+++ b/src/samples/FullFramework/iXlsxWriter.ConsoleApp/Output/Sample-01/Sample-01.xlsx
@@ -52,26 +52,21 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0"/>
+    <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0"/>
-    <xf numFmtId="49" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" xfId="1" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+  <cellXfs count="4">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="1" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="2" applyProtection="1"/>
     <xf numFmtId="49" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" xfId="2" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="31ycbfhm" xfId="1"/>
-    <cellStyle name="31ycbfhm_Alternate" xfId="2"/>
+    <cellStyle name="ya5jgkqk" xfId="1"/>
+    <cellStyle name="ya5jgkqk_Alternate" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
@@ -86,13 +81,11 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.787400" right="0.787400" top="0.787400" bottom="0.787400" header="0.315" footer="0.315"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add more Insert/Set actions, refactor and minor changes, in progress...
</commit_message>
<xml_diff>
--- a/src/samples/FullFramework/iXlsxWriter.ConsoleApp/Output/Sample-01/Sample-01.xlsx
+++ b/src/samples/FullFramework/iXlsxWriter.ConsoleApp/Output/Sample-01/Sample-01.xlsx
@@ -7,6 +7,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Sheet1'!$A$1</definedName>
+  </definedNames>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -65,8 +68,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="ya5jgkqk" xfId="1"/>
-    <cellStyle name="ya5jgkqk_Alternate" xfId="2"/>
+    <cellStyle name="dsfssm3q" xfId="1"/>
+    <cellStyle name="dsfssm3q_Alternate" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
@@ -79,6 +82,9 @@
     <sheetView workbookViewId="0" showGridLines="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="1" width="27.2543334960938" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="s">
@@ -86,6 +92,8 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.787400" right="0.787400" top="0.787400" bottom="0.787400" header="0.315" footer="0.315"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add models, documentation, samples, in progress...
</commit_message>
<xml_diff>
--- a/src/samples/FullFramework/iXlsxWriter.ConsoleApp/Output/Sample-01/Sample-01.xlsx
+++ b/src/samples/FullFramework/iXlsxWriter.ConsoleApp/Output/Sample-01/Sample-01.xlsx
@@ -68,8 +68,8 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="dsfssm3q" xfId="1"/>
-    <cellStyle name="dsfssm3q_Alternate" xfId="2"/>
+    <cellStyle name="2cst1do4" xfId="1"/>
+    <cellStyle name="2cst1do4_Alternate" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>

</xml_diff>